<commit_message>
fixed implicit and explicit waits
</commit_message>
<xml_diff>
--- a/target/classes/data/DataTest.xlsx
+++ b/target/classes/data/DataTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Address" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Bayerische Straße 25</t>
+    <t>Bayerische Strasse 25</t>
   </si>
   <si>
     <t>Bayerische Straße 25, Berlin</t>
@@ -22,8 +22,7 @@
     <t>Düsseldorfer Straße 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Düsseldorfer Straße 3, Berlin
-</t>
+    <t>Düsseldorfer Straße 3, Berlin</t>
   </si>
 </sst>
 </file>
@@ -36,11 +35,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,8 +281,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="33.43"/>
-    <col customWidth="1" min="2" max="2" width="32.57"/>
+    <col customWidth="1" min="1" max="1" width="20.71"/>
+    <col customWidth="1" min="2" max="2" width="28.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -294,7 +293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -302,7 +301,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="19.5" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>